<commit_message>
added table and range classes
</commit_message>
<xml_diff>
--- a/test/data/example-1.xlsx
+++ b/test/data/example-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heavy\projects\sheetutils\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B067F867-91E8-4D97-B528-C8A434D66264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D850A22-A0D2-44FF-BCEE-DF62FF30700A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38805" yWindow="1110" windowWidth="19575" windowHeight="18885" xr2:uid="{F3271C92-6D7A-4C64-B36B-06F98E9566A7}"/>
+    <workbookView xWindow="60390" yWindow="9720" windowWidth="16170" windowHeight="10680" xr2:uid="{F3271C92-6D7A-4C64-B36B-06F98E9566A7}"/>
   </bookViews>
   <sheets>
     <sheet name="table" sheetId="1" r:id="rId1"/>
@@ -37,19 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>evens</t>
-  </si>
-  <si>
-    <t>numbers</t>
-  </si>
-  <si>
-    <t>odds</t>
-  </si>
-  <si>
-    <t>names</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
   <si>
     <t>john</t>
   </si>
@@ -69,9 +57,6 @@
     <t>kristen</t>
   </si>
   <si>
-    <t>tammy</t>
-  </si>
-  <si>
     <t>tricky</t>
   </si>
   <si>
@@ -85,6 +70,18 @@
   </si>
   <si>
     <t>birth_date</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>odd</t>
+  </si>
+  <si>
+    <t>even</t>
+  </si>
+  <si>
+    <t>number</t>
   </si>
 </sst>
 </file>
@@ -447,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2B27A6-E8AF-4B3A-B416-737286FE8579}">
-  <dimension ref="B2:G12"/>
+  <dimension ref="B2:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,22 +458,22 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -490,7 +487,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F3" s="1">
         <v>13.34</v>
@@ -510,7 +507,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F4" s="1">
         <v>15.67</v>
@@ -530,7 +527,7 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F5" s="1">
         <v>18</v>
@@ -550,7 +547,7 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F6" s="1">
         <v>20.329999999999998</v>
@@ -570,7 +567,7 @@
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F7" s="1">
         <v>22.66</v>
@@ -589,9 +586,6 @@
       <c r="D8">
         <v>11</v>
       </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
       <c r="F8" s="1">
         <v>24.99</v>
       </c>
@@ -610,7 +604,7 @@
         <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F9" s="1">
         <v>27.32</v>
@@ -630,7 +624,7 @@
         <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F10" s="1">
         <v>29.65</v>
@@ -650,7 +644,7 @@
         <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F11" s="1">
         <v>31.98</v>
@@ -670,12 +664,406 @@
         <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F12" s="1">
         <v>34.31</v>
       </c>
       <c r="G12" s="2">
+        <v>27140</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>13.34</v>
+      </c>
+      <c r="G13" s="2">
+        <v>20070</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>15.67</v>
+      </c>
+      <c r="G14" s="2">
+        <v>34338</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="1">
+        <v>18</v>
+      </c>
+      <c r="G15" s="2">
+        <v>37502</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="1">
+        <v>20.329999999999998</v>
+      </c>
+      <c r="G16" s="2">
+        <v>41004</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="1">
+        <v>22.66</v>
+      </c>
+      <c r="G17" s="2">
+        <v>27140</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>12</v>
+      </c>
+      <c r="D18">
+        <v>11</v>
+      </c>
+      <c r="F18" s="1">
+        <v>24.99</v>
+      </c>
+      <c r="G18" s="2">
+        <v>20070</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>14</v>
+      </c>
+      <c r="D19">
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="1">
+        <v>27.32</v>
+      </c>
+      <c r="G19" s="2">
+        <v>34338</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>16</v>
+      </c>
+      <c r="D20">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="1">
+        <v>29.65</v>
+      </c>
+      <c r="G20" s="2">
+        <v>37502</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <v>18</v>
+      </c>
+      <c r="D21">
+        <v>17</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="1">
+        <v>31.98</v>
+      </c>
+      <c r="G21" s="2">
+        <v>41004</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>20</v>
+      </c>
+      <c r="D22">
+        <v>19</v>
+      </c>
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="1">
+        <v>34.31</v>
+      </c>
+      <c r="G22" s="2">
+        <v>27140</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>13.34</v>
+      </c>
+      <c r="G23" s="2">
+        <v>20070</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1">
+        <v>15.67</v>
+      </c>
+      <c r="G24" s="2">
+        <v>34338</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>6</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="1">
+        <v>18</v>
+      </c>
+      <c r="G25" s="2">
+        <v>37502</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <v>8</v>
+      </c>
+      <c r="D26">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="1">
+        <v>20.329999999999998</v>
+      </c>
+      <c r="G26" s="2">
+        <v>41004</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="1">
+        <v>22.66</v>
+      </c>
+      <c r="G27" s="2">
+        <v>27140</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>6</v>
+      </c>
+      <c r="C28">
+        <v>12</v>
+      </c>
+      <c r="D28">
+        <v>11</v>
+      </c>
+      <c r="F28" s="1">
+        <v>24.99</v>
+      </c>
+      <c r="G28" s="2">
+        <v>20070</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <v>14</v>
+      </c>
+      <c r="D29">
+        <v>13</v>
+      </c>
+      <c r="E29" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="1">
+        <v>27.32</v>
+      </c>
+      <c r="G29" s="2">
+        <v>34338</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>16</v>
+      </c>
+      <c r="D30">
+        <v>15</v>
+      </c>
+      <c r="E30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="1">
+        <v>29.65</v>
+      </c>
+      <c r="G30" s="2">
+        <v>37502</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>9</v>
+      </c>
+      <c r="C31">
+        <v>18</v>
+      </c>
+      <c r="D31">
+        <v>17</v>
+      </c>
+      <c r="E31" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="1">
+        <v>31.98</v>
+      </c>
+      <c r="G31" s="2">
+        <v>41004</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>10</v>
+      </c>
+      <c r="C32">
+        <v>20</v>
+      </c>
+      <c r="D32">
+        <v>19</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="1">
+        <v>34.31</v>
+      </c>
+      <c r="G32" s="2">
         <v>27140</v>
       </c>
     </row>

</xml_diff>